<commit_message>
Sample test case updated
</commit_message>
<xml_diff>
--- a/ConfigurationFolder/sampleTestScript/TestData.xlsx
+++ b/ConfigurationFolder/sampleTestScript/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>End</t>
   </si>
@@ -109,13 +109,25 @@
   </si>
   <si>
     <t>amazonitemadd</t>
+  </si>
+  <si>
+    <t>Fire TV</t>
+  </si>
+  <si>
+    <t>Fire TV Cube</t>
+  </si>
+  <si>
+    <t>fisrt slide bar</t>
+  </si>
+  <si>
+    <t>second slide bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +140,13 @@
       <color indexed="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -162,6 +181,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,9 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -489,7 +514,7 @@
     <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -501,28 +526,45 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:5">
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>